<commit_message>
Update all the Excel file paths to save results in the "Results" folder and update the final experiment sheet filename.
</commit_message>
<xml_diff>
--- a/Results/DT_Freq_CV_results.xlsx
+++ b/Results/DT_Freq_CV_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -643,426 +643,6 @@
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Freq</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>DecisionTreeClassifier</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>{'criterion': 'gini', 'max_depth': 15, 'min_samples_leaf': 2, 'min_samples_split': 20}</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>CV=11</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>61.40%</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>63.05%</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>61.40%</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>61.25%</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Freq</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>DecisionTreeClassifier</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>{'criterion': 'entropy', 'max_depth': 15, 'min_samples_leaf': 8, 'min_samples_split': 2}</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>CV=13</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>61.16%</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>62.82%</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>61.16%</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>60.96%</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Freq</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>DecisionTreeClassifier</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>{'criterion': 'gini', 'max_depth': 5, 'min_samples_leaf': 4, 'min_samples_split': 20}</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>CV=15</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>61.23%</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>62.13%</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>61.23%</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>60.88%</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Freq</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>DecisionTreeClassifier</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>{'criterion': 'entropy', 'max_depth': 5, 'min_samples_leaf': 4, 'min_samples_split': 20}</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>CV=17</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>62.18%</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>63.19%</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>62.18%</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>61.07%</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Freq</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>DecisionTreeClassifier</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>{'criterion': 'entropy', 'max_depth': 10, 'min_samples_leaf': 4, 'min_samples_split': 20}</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>CV=19</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>64.57%</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>65.90%</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>64.57%</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>64.34%</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Freq</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>DecisionTreeClassifier</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>{'criterion': 'gini', 'max_depth': 5, 'min_samples_leaf': 2, 'min_samples_split': 20}</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>CV=21</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>62.95%</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>65.40%</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>62.95%</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>62.52%</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Freq</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>DecisionTreeClassifier</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>{'criterion': 'gini', 'max_depth': 5, 'min_samples_leaf': 2, 'min_samples_split': 20}</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>CV=23</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>62.79%</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>65.42%</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>62.79%</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>62.47%</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Freq</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>DecisionTreeClassifier</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>{'criterion': 'gini', 'max_depth': 5, 'min_samples_leaf': 4, 'min_samples_split': 20}</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>CV=25</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>62.85%</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>66.39%</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>62.85%</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>62.62%</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Freq</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>DecisionTreeClassifier</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>{'criterion': 'gini', 'max_depth': 5, 'min_samples_leaf': 4, 'min_samples_split': 15}</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>CV=27</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>61.61%</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>63.40%</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>61.61%</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>60.98%</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Freq</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>DecisionTreeClassifier</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>{'criterion': 'gini', 'max_depth': 5, 'min_samples_leaf': 4, 'min_samples_split': 2}</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>CV=29</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>63.26%</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>66.19%</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>63.26%</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>62.95%</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update CV=9 in KFold and GridSearchCV for Decision Tree and SVM
</commit_message>
<xml_diff>
--- a/Results/DT_Freq_CV_results.xlsx
+++ b/Results/DT_Freq_CV_results.xlsx
@@ -488,7 +488,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'criterion': 'gini', 'max_depth': 15, 'min_samples_leaf': 4, 'min_samples_split': 20}</t>
+          <t>{'criterion': 'gini', 'max_depth': 5, 'min_samples_leaf': 4, 'min_samples_split': 2}</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -498,22 +498,22 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>60.59%</t>
+          <t>58.99%</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>61.91%</t>
+          <t>60.27%</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>60.59%</t>
+          <t>58.99%</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>60.41%</t>
+          <t>58.42%</t>
         </is>
       </c>
     </row>

</xml_diff>